<commit_message>
Adding lab 22 and 23
</commit_message>
<xml_diff>
--- a/22_cardiac_arrest/22_cardiac_arrest_data.xlsx
+++ b/22_cardiac_arrest/22_cardiac_arrest_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="9525"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20730" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>Blood Pressure(mmHg)</t>
   </si>
   <si>
-    <t>123/78</t>
-  </si>
-  <si>
     <t>13/13</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>Symp Activity(Hz)</t>
+  </si>
+  <si>
+    <t>124/79</t>
   </si>
 </sst>
 </file>
@@ -482,21 +482,21 @@
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="75.75" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
-        <v>5361</v>
+        <v>5346</v>
       </c>
       <c r="C4" s="4">
         <v>0</v>
@@ -507,13 +507,13 @@
     </row>
     <row r="5" spans="1:4" ht="45.75" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
-        <v>6.8</v>
+        <v>6.5</v>
       </c>
       <c r="C5" s="4">
-        <v>0</v>
+        <v>54.3</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -521,13 +521,13 @@
     </row>
     <row r="6" spans="1:4" ht="45.75" thickBot="1">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4">
         <v>1.5</v>
       </c>
       <c r="C6" s="4">
-        <v>13.8</v>
+        <v>14</v>
       </c>
       <c r="D6" s="4">
         <v>16.8</v>

</xml_diff>

<commit_message>
Adding Lab 22 HumMod data. However, a divide by zero error that cannot be avoided prevents the lab from being completed.
</commit_message>
<xml_diff>
--- a/22_cardiac_arrest/22_cardiac_arrest_data.xlsx
+++ b/22_cardiac_arrest/22_cardiac_arrest_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Cardiac Arrest</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>124/79</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>120/79</t>
+  </si>
+  <si>
+    <t>Patient does not reach 30 seconds before a divide by zero error in Structure\CO\CO.DES occurs The variable involved is Bronchi[CO] - (Uptake / Breathing.AlveolarVentilation(STPD))</t>
   </si>
 </sst>
 </file>
@@ -70,12 +82,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -142,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -155,6 +173,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,20 +474,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -476,8 +509,20 @@
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="60.75" thickBot="1">
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="60.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -490,8 +535,16 @@
       <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="75.75" thickBot="1">
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" ht="75.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -504,8 +557,16 @@
       <c r="D4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="45.75" thickBot="1">
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="4">
+        <v>5468</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" ht="45.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -518,8 +579,16 @@
       <c r="D5" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="45.75" thickBot="1">
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4">
+        <v>6.6</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" ht="45.75" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -532,8 +601,54 @@
       <c r="D6" s="4">
         <v>16.8</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:I10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>